<commit_message>
Best performing models update
</commit_message>
<xml_diff>
--- a/report/12hr_OverviewModelPerformance.xlsx
+++ b/report/12hr_OverviewModelPerformance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="29">
   <si>
     <t xml:space="preserve">All Features</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">Recall Test Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youden's Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPR Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPR Test</t>
   </si>
   <si>
     <t xml:space="preserve">KNN</t>
@@ -188,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,12 +254,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -338,10 +351,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -352,12 +365,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,8 +382,11 @@
       <c r="D1" s="7"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="K1" s="0"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
     </row>
     <row r="2" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -391,18 +407,27 @@
       <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="0"/>
+      <c r="G2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L2" s="0"/>
-    </row>
-    <row r="3" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="0"/>
+    </row>
+    <row r="3" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>0.87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" s="13" t="n">
         <v>0.799221357063404</v>
@@ -413,21 +438,29 @@
       <c r="F3" s="13" t="n">
         <v>0.81</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="0"/>
+      <c r="G3" s="13" t="n">
+        <v>0.451612903225807</v>
+      </c>
+      <c r="H3" s="14" t="n">
+        <v>0.5483871</v>
+      </c>
+      <c r="I3" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="0"/>
-    </row>
-    <row r="4" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
-        <v>9</v>
+      <c r="M3" s="0"/>
+    </row>
+    <row r="4" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="12" t="n">
         <v>0.9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="13" t="n">
         <v>0.865406006674082</v>
@@ -438,21 +471,29 @@
       <c r="F4" s="13" t="n">
         <v>0.909</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="0"/>
+      <c r="G4" s="13" t="n">
+        <v>0.610678531701891</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0.35483871</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <v>0.96551724</v>
+      </c>
+      <c r="J4" s="0"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="0"/>
-    </row>
-    <row r="5" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>11</v>
+      <c r="M4" s="0"/>
+    </row>
+    <row r="5" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="12" t="n">
         <v>0.91</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="13" t="n">
         <v>0.883203559510567</v>
@@ -463,22 +504,29 @@
       <c r="F5" s="13" t="n">
         <v>0.857</v>
       </c>
-      <c r="G5" s="0"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="0"/>
+      <c r="G5" s="13" t="n">
+        <v>0.675194660734149</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0.29032258</v>
+      </c>
+      <c r="I5" s="13" t="n">
+        <v>0.96551724</v>
+      </c>
+      <c r="J5" s="0"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="12" t="n">
         <v>0.89</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" s="13" t="n">
         <v>0.81979977753059</v>
@@ -489,18 +537,26 @@
       <c r="F6" s="13" t="n">
         <v>0.724</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="G6" s="13" t="n">
+        <v>0.546162402669633</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0.41935484</v>
+      </c>
+      <c r="I6" s="13" t="n">
+        <v>0.96551724</v>
+      </c>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>14</v>
+      <c r="A7" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="12" t="n">
         <v>0.9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D7" s="13" t="n">
         <v>0.839822024471635</v>
@@ -511,21 +567,29 @@
       <c r="F7" s="13" t="n">
         <v>0.84</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="G7" s="13" t="n">
+        <v>0.576195773081201</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0.35483871</v>
+      </c>
+      <c r="I7" s="13" t="n">
+        <v>0.93103448</v>
+      </c>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" s="13" t="n">
         <v>0.677</v>
@@ -533,19 +597,28 @@
       <c r="F8" s="13" t="n">
         <v>0.84</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" s="13" t="n">
         <v>0.677</v>
@@ -553,16 +626,25 @@
       <c r="F9" s="13" t="n">
         <v>0.913</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" s="13" t="n">
         <v>0.860956618464961</v>
@@ -573,16 +655,25 @@
       <c r="F10" s="13" t="n">
         <v>0.846</v>
       </c>
+      <c r="G10" s="13" t="n">
+        <v>0.60845383759733</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0.06896552</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0.67741935</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11" s="13" t="n">
         <v>0.853170189098999</v>
@@ -593,16 +684,25 @@
       <c r="F11" s="13" t="n">
         <v>0.852</v>
       </c>
+      <c r="G11" s="13" t="n">
+        <v>0.64071190211346</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0.06896552</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>0.70967742</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D12" s="13" t="n">
         <v>0.869855394883204</v>
@@ -613,10 +713,19 @@
       <c r="F12" s="13" t="n">
         <v>0.92</v>
       </c>
+      <c r="G12" s="13" t="n">
+        <v>0.672969966629589</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>0.06896552</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>0.74193548</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -639,205 +748,304 @@
       <c r="F15" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="G15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="B16" s="18" t="n">
         <v>0.88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="13" t="n">
         <v>0.827586206896552</v>
       </c>
-      <c r="E16" s="15" t="n">
+      <c r="E16" s="13" t="n">
         <v>0.645</v>
       </c>
-      <c r="F16" s="15" t="n">
+      <c r="F16" s="13" t="n">
         <v>0.8</v>
+      </c>
+      <c r="G16" s="13" t="n">
+        <v>0.472747497219132</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>0.35483871</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>0.82758621</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>0.84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="15" t="n">
+        <v>26</v>
+      </c>
+      <c r="D17" s="13" t="n">
         <v>0.735261401557286</v>
       </c>
-      <c r="E17" s="15" t="n">
+      <c r="E17" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F17" s="15" t="n">
+      <c r="F17" s="13" t="n">
         <v>0.733</v>
       </c>
+      <c r="G17" s="13" t="n">
+        <v>0.46384872080089</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>0.22580645</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>0.68965517</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>11</v>
+      <c r="A18" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>0.91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D18" s="13" t="n">
         <v>0.883203559510567</v>
       </c>
-      <c r="E18" s="15" t="n">
+      <c r="E18" s="13" t="n">
         <v>0.774</v>
       </c>
-      <c r="F18" s="15" t="n">
+      <c r="F18" s="13" t="n">
         <v>0.857</v>
       </c>
+      <c r="G18" s="13" t="n">
+        <v>0.675194660734149</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>0.29032258</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>0.96551724</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>13</v>
+      <c r="A19" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>0.89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="D19" s="13" t="n">
         <v>0.813125695216908</v>
       </c>
-      <c r="E19" s="15" t="n">
+      <c r="E19" s="13" t="n">
         <v>0.677</v>
       </c>
-      <c r="F19" s="15" t="n">
+      <c r="F19" s="13" t="n">
         <v>0.724</v>
       </c>
+      <c r="G19" s="13" t="n">
+        <v>0.513904338153504</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>0.4516129</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>0.96551724</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>14</v>
+      <c r="A20" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>0.91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="15" t="n">
+        <v>27</v>
+      </c>
+      <c r="D20" s="13" t="n">
         <v>0.826473859844271</v>
       </c>
-      <c r="E20" s="15" t="n">
+      <c r="E20" s="13" t="n">
         <v>0.645</v>
       </c>
-      <c r="F20" s="15" t="n">
+      <c r="F20" s="13" t="n">
         <v>0.87</v>
+      </c>
+      <c r="G20" s="13" t="n">
+        <v>0.548387096774194</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>0.4516129</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" s="13" t="n">
         <v>0.677</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="F21" s="13" t="n">
         <v>0.808</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="F22" s="13" t="n">
         <v>0.815</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D23" s="13" t="n">
         <v>0.844271412680756</v>
       </c>
-      <c r="E23" s="15" t="n">
+      <c r="E23" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F23" s="15" t="n">
+      <c r="F23" s="13" t="n">
         <v>0.846</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>0.604004449388209</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>0.13793103</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <v>0.74193548</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D24" s="13" t="n">
         <v>0.853170189098999</v>
       </c>
-      <c r="E24" s="15" t="n">
+      <c r="E24" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F24" s="15" t="n">
+      <c r="F24" s="13" t="n">
         <v>0.846</v>
+      </c>
+      <c r="G24" s="13" t="n">
+        <v>0.60622914349277</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>0.10344828</v>
+      </c>
+      <c r="I24" s="3" t="n">
+        <v>0.70967742</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D25" s="13" t="n">
         <v>0.849833147942158</v>
       </c>
-      <c r="E25" s="15" t="n">
+      <c r="E25" s="13" t="n">
         <v>0.742</v>
       </c>
-      <c r="F25" s="15" t="n">
+      <c r="F25" s="13" t="n">
         <v>0.821</v>
+      </c>
+      <c r="G25" s="13" t="n">
+        <v>0.638487208008899</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>0.10344828</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <v>0.74193548</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,7 +1053,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -868,205 +1076,304 @@
       <c r="F28" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="G28" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="B29" s="18" t="n">
         <v>0.87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="D29" s="13" t="n">
         <v>0.805339265850945</v>
       </c>
-      <c r="E29" s="15" t="n">
+      <c r="E29" s="13" t="n">
         <v>0.581</v>
       </c>
-      <c r="F29" s="15" t="n">
+      <c r="F29" s="13" t="n">
         <v>0.783</v>
       </c>
+      <c r="G29" s="13" t="n">
+        <v>0.451612903225807</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>0.5483871</v>
+      </c>
+      <c r="I29" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="s">
-        <v>9</v>
+      <c r="A30" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>0.9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="D30" s="13" t="n">
         <v>0.862068965517241</v>
       </c>
-      <c r="E30" s="15" t="n">
+      <c r="E30" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F30" s="15" t="n">
+      <c r="F30" s="13" t="n">
         <v>0.815</v>
       </c>
+      <c r="G30" s="13" t="n">
+        <v>0.64293659621802</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>0.32258065</v>
+      </c>
+      <c r="I30" s="3" t="n">
+        <v>0.96551724</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="s">
-        <v>11</v>
+      <c r="A31" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>0.91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D31" s="13" t="n">
         <v>0.883203559510567</v>
       </c>
-      <c r="E31" s="15" t="n">
+      <c r="E31" s="13" t="n">
         <v>0.774</v>
       </c>
-      <c r="F31" s="15" t="n">
+      <c r="F31" s="13" t="n">
         <v>0.857</v>
+      </c>
+      <c r="G31" s="13" t="n">
+        <v>0.675194660734149</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>0.29032258</v>
+      </c>
+      <c r="I31" s="3" t="n">
+        <v>0.96551724</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>0.89</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="D32" s="13" t="n">
         <v>0.81979977753059</v>
       </c>
-      <c r="E32" s="15" t="n">
+      <c r="E32" s="13" t="n">
         <v>0.677</v>
       </c>
-      <c r="F32" s="15" t="n">
+      <c r="F32" s="13" t="n">
         <v>0.75</v>
       </c>
+      <c r="G32" s="13" t="n">
+        <v>0.516129032258065</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>0.48387097</v>
+      </c>
+      <c r="I32" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16" t="s">
-        <v>14</v>
+      <c r="A33" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>0.91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="15" t="n">
+        <v>27</v>
+      </c>
+      <c r="D33" s="13" t="n">
         <v>0.830923248053393</v>
       </c>
-      <c r="E33" s="15" t="n">
+      <c r="E33" s="13" t="n">
         <v>0.645</v>
       </c>
-      <c r="F33" s="15" t="n">
+      <c r="F33" s="13" t="n">
         <v>0.87</v>
+      </c>
+      <c r="G33" s="13" t="n">
+        <v>0.60622914349277</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>0.29032258</v>
+      </c>
+      <c r="I33" s="3" t="n">
+        <v>0.89655172</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E34" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F34" s="15" t="n">
+      <c r="F34" s="13" t="n">
         <v>0.846</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E35" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F35" s="15" t="n">
+      <c r="F35" s="13" t="n">
         <v>0.88</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D36" s="13" t="n">
         <v>0.854282536151279</v>
       </c>
-      <c r="E36" s="15" t="n">
+      <c r="E36" s="13" t="n">
         <v>0.71</v>
       </c>
-      <c r="F36" s="15" t="n">
+      <c r="F36" s="13" t="n">
         <v>0.846</v>
+      </c>
+      <c r="G36" s="13" t="n">
+        <v>0.60845383759733</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>0.06896552</v>
+      </c>
+      <c r="I36" s="3" t="n">
+        <v>0.67741935</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D37" s="13" t="n">
         <v>0.854282536151279</v>
       </c>
-      <c r="E37" s="15" t="n">
+      <c r="E37" s="13" t="n">
         <v>0.742</v>
       </c>
-      <c r="F37" s="15" t="n">
+      <c r="F37" s="13" t="n">
         <v>0.885</v>
+      </c>
+      <c r="G37" s="13" t="n">
+        <v>0.672969966629589</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>0.06896552</v>
+      </c>
+      <c r="I37" s="3" t="n">
+        <v>0.74193548</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D38" s="13" t="n">
         <v>0.863181312569522</v>
       </c>
-      <c r="E38" s="15" t="n">
+      <c r="E38" s="13" t="n">
         <v>0.742</v>
       </c>
-      <c r="F38" s="15" t="n">
+      <c r="F38" s="13" t="n">
         <v>0.92</v>
+      </c>
+      <c r="G38" s="13" t="n">
+        <v>0.672969966629589</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>0.06896552</v>
+      </c>
+      <c r="I38" s="3" t="n">
+        <v>0.74193548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>